<commit_message>
updating database with new data from students
</commit_message>
<xml_diff>
--- a/Hier_MainDB.xlsx
+++ b/Hier_MainDB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studugedu-my.sharepoint.com/personal/m_witkowska_ug_edu_pl/Documents/Dydaktyka/Ekologia zwierząt/Biologia/Park Oliwski/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studugedu-my.sharepoint.com/personal/m_witkowska_ug_edu_pl/Documents/Dydaktyka/Ekologia zwierząt/Animal-Ecology-Lab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1041" documentId="8_{2CF9D3AD-E501-42C8-8B0C-2C1FDDFD0CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3C5FD39E-F11B-4F90-B902-B364E2F47258}"/>
+  <xr:revisionPtr revIDLastSave="1109" documentId="8_{2CF9D3AD-E501-42C8-8B0C-2C1FDDFD0CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2B75748-6534-44F7-9340-C4A25324CEA5}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26232" yWindow="-1056" windowWidth="23016" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hierarchia" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="19">
   <si>
     <t>ZJAD</t>
   </si>
@@ -102,7 +102,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,6 +155,24 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -164,7 +182,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -172,12 +190,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -185,6 +212,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -201,10 +247,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -504,23 +546,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T39"/>
+  <dimension ref="A1:T75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S8" sqref="S8"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q72" sqref="Q72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.08984375" style="3"/>
+    <col min="1" max="1" width="9.109375" style="3"/>
     <col min="2" max="2" width="11" style="3" customWidth="1"/>
-    <col min="3" max="3" width="9.08984375" style="3"/>
-    <col min="4" max="4" width="9.54296875" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="9.08984375" style="3"/>
+    <col min="3" max="3" width="9.109375" style="3"/>
+    <col min="4" max="4" width="9.5546875" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -572,7 +614,7 @@
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -622,7 +664,7 @@
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -672,7 +714,7 @@
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -722,7 +764,7 @@
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -772,7 +814,7 @@
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -822,7 +864,7 @@
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -872,7 +914,7 @@
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -916,7 +958,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -960,7 +1002,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1004,7 +1046,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1048,7 +1090,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1092,7 +1134,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1136,7 +1178,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1180,7 +1222,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1224,7 +1266,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1268,7 +1310,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1312,7 +1354,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1356,7 +1398,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1400,7 +1442,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1444,7 +1486,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1488,7 +1530,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1526,7 +1568,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -1567,7 +1609,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1605,7 +1647,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -1646,7 +1688,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1684,7 +1726,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -1725,7 +1767,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -1759,7 +1801,7 @@
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -1793,7 +1835,7 @@
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -1831,7 +1873,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -1872,7 +1914,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -1900,7 +1942,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -1938,7 +1980,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -1976,7 +2018,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -2004,7 +2046,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -2042,7 +2084,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -2080,7 +2122,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -2118,7 +2160,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -2156,6 +2198,1387 @@
         <v>12</v>
       </c>
       <c r="O39" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A40" s="2">
+        <v>39</v>
+      </c>
+      <c r="B40" s="7">
+        <v>35</v>
+      </c>
+      <c r="C40" s="7">
+        <v>0</v>
+      </c>
+      <c r="D40" s="7">
+        <v>1</v>
+      </c>
+      <c r="E40" s="7">
+        <v>3</v>
+      </c>
+      <c r="F40" s="7">
+        <v>4</v>
+      </c>
+      <c r="G40" s="7">
+        <v>3</v>
+      </c>
+      <c r="H40" s="7">
+        <v>3</v>
+      </c>
+      <c r="I40" s="7">
+        <v>2</v>
+      </c>
+      <c r="J40" s="7">
+        <v>3</v>
+      </c>
+      <c r="N40" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O40" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A41" s="2">
+        <v>40</v>
+      </c>
+      <c r="B41" s="7">
+        <v>90</v>
+      </c>
+      <c r="C41" s="7">
+        <v>1</v>
+      </c>
+      <c r="D41" s="7">
+        <v>0</v>
+      </c>
+      <c r="E41" s="7">
+        <v>1</v>
+      </c>
+      <c r="F41" s="7">
+        <v>11</v>
+      </c>
+      <c r="G41" s="7">
+        <v>2</v>
+      </c>
+      <c r="H41" s="7">
+        <v>2</v>
+      </c>
+      <c r="I41" s="7">
+        <v>2</v>
+      </c>
+      <c r="J41" s="7">
+        <v>1</v>
+      </c>
+      <c r="N41" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O41" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A42" s="2">
+        <v>41</v>
+      </c>
+      <c r="B42" s="7">
+        <v>60</v>
+      </c>
+      <c r="C42" s="7">
+        <v>1</v>
+      </c>
+      <c r="D42" s="7">
+        <v>0</v>
+      </c>
+      <c r="E42" s="7">
+        <v>2</v>
+      </c>
+      <c r="F42" s="7">
+        <v>1</v>
+      </c>
+      <c r="G42" s="7">
+        <v>3</v>
+      </c>
+      <c r="H42" s="7">
+        <v>3</v>
+      </c>
+      <c r="I42" s="7">
+        <v>3</v>
+      </c>
+      <c r="J42" s="7">
+        <v>3</v>
+      </c>
+      <c r="N42" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O42" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A43" s="2">
+        <v>42</v>
+      </c>
+      <c r="B43" s="7">
+        <v>51</v>
+      </c>
+      <c r="C43" s="7">
+        <v>1</v>
+      </c>
+      <c r="D43" s="7">
+        <v>5</v>
+      </c>
+      <c r="E43" s="7">
+        <v>1</v>
+      </c>
+      <c r="F43" s="7">
+        <v>0</v>
+      </c>
+      <c r="G43" s="7">
+        <v>2</v>
+      </c>
+      <c r="H43" s="7">
+        <v>3</v>
+      </c>
+      <c r="I43" s="7">
+        <v>2</v>
+      </c>
+      <c r="J43" s="7">
+        <v>3</v>
+      </c>
+      <c r="N43" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O43" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A44" s="2">
+        <v>43</v>
+      </c>
+      <c r="B44" s="8">
+        <v>98</v>
+      </c>
+      <c r="C44" s="8">
+        <v>2</v>
+      </c>
+      <c r="D44" s="8">
+        <v>2</v>
+      </c>
+      <c r="E44" s="8">
+        <v>3</v>
+      </c>
+      <c r="F44" s="8">
+        <v>0</v>
+      </c>
+      <c r="G44" s="8">
+        <v>1</v>
+      </c>
+      <c r="H44" s="8">
+        <v>2</v>
+      </c>
+      <c r="I44" s="8">
+        <v>1</v>
+      </c>
+      <c r="J44" s="8">
+        <v>1</v>
+      </c>
+      <c r="N44" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O44" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A45" s="2">
+        <v>44</v>
+      </c>
+      <c r="B45" s="9">
+        <v>1</v>
+      </c>
+      <c r="C45" s="9">
+        <v>0</v>
+      </c>
+      <c r="D45" s="9">
+        <v>0</v>
+      </c>
+      <c r="E45" s="9">
+        <v>3</v>
+      </c>
+      <c r="F45" s="9">
+        <v>12</v>
+      </c>
+      <c r="G45" s="9">
+        <v>3</v>
+      </c>
+      <c r="H45" s="9">
+        <v>3</v>
+      </c>
+      <c r="I45" s="9">
+        <v>3</v>
+      </c>
+      <c r="J45" s="9">
+        <v>3</v>
+      </c>
+      <c r="N45" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O45" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A46" s="2">
+        <v>45</v>
+      </c>
+      <c r="B46" s="9">
+        <v>129</v>
+      </c>
+      <c r="C46" s="9">
+        <v>3</v>
+      </c>
+      <c r="D46" s="9">
+        <v>12</v>
+      </c>
+      <c r="E46" s="9">
+        <v>4</v>
+      </c>
+      <c r="F46" s="9">
+        <v>8</v>
+      </c>
+      <c r="G46" s="9">
+        <v>2</v>
+      </c>
+      <c r="H46" s="9">
+        <v>1</v>
+      </c>
+      <c r="I46" s="9">
+        <v>1</v>
+      </c>
+      <c r="J46" s="9">
+        <v>1</v>
+      </c>
+      <c r="N46" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O46" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A47" s="2">
+        <v>46</v>
+      </c>
+      <c r="B47" s="9">
+        <v>29</v>
+      </c>
+      <c r="C47" s="9">
+        <v>4</v>
+      </c>
+      <c r="D47" s="9">
+        <v>8</v>
+      </c>
+      <c r="E47" s="9">
+        <v>1</v>
+      </c>
+      <c r="F47" s="9">
+        <v>0</v>
+      </c>
+      <c r="G47" s="9">
+        <v>3</v>
+      </c>
+      <c r="H47" s="9">
+        <v>3</v>
+      </c>
+      <c r="I47" s="9">
+        <v>3</v>
+      </c>
+      <c r="J47" s="9">
+        <v>3</v>
+      </c>
+      <c r="N47" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O47" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A48" s="2">
+        <v>47</v>
+      </c>
+      <c r="B48" s="9">
+        <v>360</v>
+      </c>
+      <c r="C48" s="9">
+        <v>3</v>
+      </c>
+      <c r="D48" s="9">
+        <v>8</v>
+      </c>
+      <c r="E48" s="9">
+        <v>5</v>
+      </c>
+      <c r="F48" s="9">
+        <v>4</v>
+      </c>
+      <c r="G48" s="9">
+        <v>1</v>
+      </c>
+      <c r="H48" s="9">
+        <v>1</v>
+      </c>
+      <c r="I48" s="9">
+        <v>1</v>
+      </c>
+      <c r="J48" s="9">
+        <v>1</v>
+      </c>
+      <c r="N48" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O48" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A49" s="2">
+        <v>48</v>
+      </c>
+      <c r="B49" s="10">
+        <v>0</v>
+      </c>
+      <c r="C49" s="10">
+        <v>0</v>
+      </c>
+      <c r="D49" s="10">
+        <v>0</v>
+      </c>
+      <c r="E49" s="10">
+        <v>1</v>
+      </c>
+      <c r="F49" s="10">
+        <v>1</v>
+      </c>
+      <c r="G49" s="10">
+        <v>1</v>
+      </c>
+      <c r="H49" s="10">
+        <v>3</v>
+      </c>
+      <c r="I49" s="10">
+        <v>1</v>
+      </c>
+      <c r="J49" s="10">
+        <v>3</v>
+      </c>
+      <c r="N49" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O49" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A50" s="2">
+        <v>49</v>
+      </c>
+      <c r="B50" s="11">
+        <v>19</v>
+      </c>
+      <c r="C50" s="11">
+        <v>1</v>
+      </c>
+      <c r="D50" s="11">
+        <v>2</v>
+      </c>
+      <c r="E50" s="11">
+        <v>4</v>
+      </c>
+      <c r="F50" s="11">
+        <v>7</v>
+      </c>
+      <c r="G50" s="11">
+        <v>3</v>
+      </c>
+      <c r="H50" s="11">
+        <v>2</v>
+      </c>
+      <c r="I50" s="11">
+        <v>1</v>
+      </c>
+      <c r="J50" s="11">
+        <v>3</v>
+      </c>
+      <c r="N50" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O50" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A51" s="2">
+        <v>50</v>
+      </c>
+      <c r="B51" s="11">
+        <v>28</v>
+      </c>
+      <c r="C51" s="11">
+        <v>7</v>
+      </c>
+      <c r="D51" s="11">
+        <v>9</v>
+      </c>
+      <c r="E51" s="11">
+        <v>5</v>
+      </c>
+      <c r="F51" s="11">
+        <v>2</v>
+      </c>
+      <c r="G51" s="11">
+        <v>3</v>
+      </c>
+      <c r="H51" s="11">
+        <v>2</v>
+      </c>
+      <c r="I51" s="11">
+        <v>1</v>
+      </c>
+      <c r="J51" s="11">
+        <v>3</v>
+      </c>
+      <c r="N51" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O51" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A52" s="2">
+        <v>51</v>
+      </c>
+      <c r="B52" s="11">
+        <v>16</v>
+      </c>
+      <c r="C52" s="11">
+        <v>0</v>
+      </c>
+      <c r="D52" s="11">
+        <v>0</v>
+      </c>
+      <c r="E52" s="11">
+        <v>2</v>
+      </c>
+      <c r="F52" s="11">
+        <v>3</v>
+      </c>
+      <c r="G52" s="11">
+        <v>3</v>
+      </c>
+      <c r="H52" s="11">
+        <v>3</v>
+      </c>
+      <c r="I52" s="11">
+        <v>3</v>
+      </c>
+      <c r="J52" s="11">
+        <v>3</v>
+      </c>
+      <c r="N52" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O52" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A53" s="2">
+        <v>52</v>
+      </c>
+      <c r="B53" s="11">
+        <v>14</v>
+      </c>
+      <c r="C53" s="11">
+        <v>1</v>
+      </c>
+      <c r="D53" s="11">
+        <v>1</v>
+      </c>
+      <c r="E53" s="11">
+        <v>0</v>
+      </c>
+      <c r="F53" s="11">
+        <v>3</v>
+      </c>
+      <c r="G53" s="11">
+        <v>3</v>
+      </c>
+      <c r="H53" s="11">
+        <v>1</v>
+      </c>
+      <c r="I53" s="11">
+        <v>3</v>
+      </c>
+      <c r="J53" s="11">
+        <v>3</v>
+      </c>
+      <c r="N53" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O53" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A54" s="2">
+        <v>53</v>
+      </c>
+      <c r="B54" s="12">
+        <v>17</v>
+      </c>
+      <c r="C54" s="12">
+        <v>4</v>
+      </c>
+      <c r="D54" s="12">
+        <v>1</v>
+      </c>
+      <c r="E54" s="12">
+        <v>2</v>
+      </c>
+      <c r="F54" s="12">
+        <v>2</v>
+      </c>
+      <c r="G54" s="12">
+        <v>3</v>
+      </c>
+      <c r="H54" s="12">
+        <v>2</v>
+      </c>
+      <c r="I54" s="12">
+        <v>2</v>
+      </c>
+      <c r="J54" s="12">
+        <v>3</v>
+      </c>
+      <c r="N54" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O54" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A55" s="2">
+        <v>54</v>
+      </c>
+      <c r="B55" s="13">
+        <v>19</v>
+      </c>
+      <c r="C55" s="13">
+        <v>1</v>
+      </c>
+      <c r="D55" s="13">
+        <v>2</v>
+      </c>
+      <c r="E55" s="13">
+        <v>4</v>
+      </c>
+      <c r="F55" s="13">
+        <v>7</v>
+      </c>
+      <c r="G55" s="13">
+        <v>3</v>
+      </c>
+      <c r="H55" s="13">
+        <v>2</v>
+      </c>
+      <c r="I55" s="13">
+        <v>1</v>
+      </c>
+      <c r="J55" s="13">
+        <v>3</v>
+      </c>
+      <c r="N55" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O55" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A56" s="2">
+        <v>55</v>
+      </c>
+      <c r="B56" s="13">
+        <v>28</v>
+      </c>
+      <c r="C56" s="13">
+        <v>7</v>
+      </c>
+      <c r="D56" s="13">
+        <v>9</v>
+      </c>
+      <c r="E56" s="13">
+        <v>5</v>
+      </c>
+      <c r="F56" s="13">
+        <v>2</v>
+      </c>
+      <c r="G56" s="13">
+        <v>3</v>
+      </c>
+      <c r="H56" s="13">
+        <v>2</v>
+      </c>
+      <c r="I56" s="13">
+        <v>1</v>
+      </c>
+      <c r="J56" s="13">
+        <v>3</v>
+      </c>
+      <c r="N56" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O56" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A57" s="2">
+        <v>56</v>
+      </c>
+      <c r="B57" s="13">
+        <v>16</v>
+      </c>
+      <c r="C57" s="13">
+        <v>0</v>
+      </c>
+      <c r="D57" s="13">
+        <v>0</v>
+      </c>
+      <c r="E57" s="13">
+        <v>2</v>
+      </c>
+      <c r="F57" s="13">
+        <v>3</v>
+      </c>
+      <c r="G57" s="13">
+        <v>3</v>
+      </c>
+      <c r="H57" s="13">
+        <v>3</v>
+      </c>
+      <c r="I57" s="13">
+        <v>3</v>
+      </c>
+      <c r="J57" s="13">
+        <v>3</v>
+      </c>
+      <c r="N57" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O57" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A58" s="2">
+        <v>57</v>
+      </c>
+      <c r="B58" s="13">
+        <v>14</v>
+      </c>
+      <c r="C58" s="13">
+        <v>1</v>
+      </c>
+      <c r="D58" s="13">
+        <v>1</v>
+      </c>
+      <c r="E58" s="13">
+        <v>0</v>
+      </c>
+      <c r="F58" s="13">
+        <v>3</v>
+      </c>
+      <c r="G58" s="13">
+        <v>3</v>
+      </c>
+      <c r="H58" s="13">
+        <v>1</v>
+      </c>
+      <c r="I58" s="13">
+        <v>3</v>
+      </c>
+      <c r="J58" s="13">
+        <v>3</v>
+      </c>
+      <c r="N58" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O58" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A59" s="2">
+        <v>58</v>
+      </c>
+      <c r="B59" s="14">
+        <v>17</v>
+      </c>
+      <c r="C59" s="14">
+        <v>4</v>
+      </c>
+      <c r="D59" s="14">
+        <v>1</v>
+      </c>
+      <c r="E59" s="14">
+        <v>2</v>
+      </c>
+      <c r="F59" s="14">
+        <v>2</v>
+      </c>
+      <c r="G59" s="14">
+        <v>3</v>
+      </c>
+      <c r="H59" s="14">
+        <v>2</v>
+      </c>
+      <c r="I59" s="14">
+        <v>2</v>
+      </c>
+      <c r="J59" s="14">
+        <v>3</v>
+      </c>
+      <c r="N59" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O59" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A60" s="2">
+        <v>59</v>
+      </c>
+      <c r="B60" s="15">
+        <v>8</v>
+      </c>
+      <c r="C60" s="15">
+        <v>2</v>
+      </c>
+      <c r="D60" s="15">
+        <v>3</v>
+      </c>
+      <c r="E60" s="15">
+        <v>6</v>
+      </c>
+      <c r="F60" s="15">
+        <v>3</v>
+      </c>
+      <c r="G60" s="15">
+        <v>2</v>
+      </c>
+      <c r="H60" s="15">
+        <v>3</v>
+      </c>
+      <c r="I60" s="15">
+        <v>1</v>
+      </c>
+      <c r="J60" s="15">
+        <v>2</v>
+      </c>
+      <c r="N60" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O60" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A61" s="2">
+        <v>60</v>
+      </c>
+      <c r="B61" s="15">
+        <v>7</v>
+      </c>
+      <c r="C61" s="15">
+        <v>0</v>
+      </c>
+      <c r="D61" s="15">
+        <v>0</v>
+      </c>
+      <c r="E61" s="15">
+        <v>0</v>
+      </c>
+      <c r="F61" s="15">
+        <v>5</v>
+      </c>
+      <c r="G61" s="15">
+        <v>3</v>
+      </c>
+      <c r="H61" s="15">
+        <v>1</v>
+      </c>
+      <c r="I61" s="15">
+        <v>3</v>
+      </c>
+      <c r="J61" s="15">
+        <v>1</v>
+      </c>
+      <c r="N61" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O61" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A62" s="2">
+        <v>61</v>
+      </c>
+      <c r="B62" s="15">
+        <v>13</v>
+      </c>
+      <c r="C62" s="15">
+        <v>0</v>
+      </c>
+      <c r="D62" s="15">
+        <v>0</v>
+      </c>
+      <c r="E62" s="15">
+        <v>2</v>
+      </c>
+      <c r="F62" s="15">
+        <v>5</v>
+      </c>
+      <c r="G62" s="15">
+        <v>3</v>
+      </c>
+      <c r="H62" s="15">
+        <v>2</v>
+      </c>
+      <c r="I62" s="15">
+        <v>2</v>
+      </c>
+      <c r="J62" s="15">
+        <v>2</v>
+      </c>
+      <c r="N62" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O62" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A63" s="2">
+        <v>62</v>
+      </c>
+      <c r="B63" s="15">
+        <v>30</v>
+      </c>
+      <c r="C63" s="15">
+        <v>0</v>
+      </c>
+      <c r="D63" s="15">
+        <v>1</v>
+      </c>
+      <c r="E63" s="15">
+        <v>1</v>
+      </c>
+      <c r="F63" s="15">
+        <v>0</v>
+      </c>
+      <c r="G63" s="15">
+        <v>2</v>
+      </c>
+      <c r="H63" s="15">
+        <v>1</v>
+      </c>
+      <c r="I63" s="15">
+        <v>2</v>
+      </c>
+      <c r="J63" s="15">
+        <v>1</v>
+      </c>
+      <c r="N63" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O63" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A64" s="2">
+        <v>63</v>
+      </c>
+      <c r="B64" s="16">
+        <v>2</v>
+      </c>
+      <c r="C64" s="16">
+        <v>1</v>
+      </c>
+      <c r="D64" s="16">
+        <v>0</v>
+      </c>
+      <c r="E64" s="16">
+        <v>0</v>
+      </c>
+      <c r="F64" s="16">
+        <v>0</v>
+      </c>
+      <c r="G64" s="16">
+        <v>3</v>
+      </c>
+      <c r="H64" s="16">
+        <v>3</v>
+      </c>
+      <c r="I64" s="16">
+        <v>3</v>
+      </c>
+      <c r="J64" s="16">
+        <v>3</v>
+      </c>
+      <c r="N64" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O64" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A65" s="2">
+        <v>64</v>
+      </c>
+      <c r="B65" s="17">
+        <v>12</v>
+      </c>
+      <c r="C65" s="18">
+        <v>2</v>
+      </c>
+      <c r="D65" s="18">
+        <v>2</v>
+      </c>
+      <c r="E65" s="17">
+        <v>0</v>
+      </c>
+      <c r="F65" s="17">
+        <v>3</v>
+      </c>
+      <c r="G65" s="17">
+        <v>2</v>
+      </c>
+      <c r="H65" s="17">
+        <v>3</v>
+      </c>
+      <c r="I65" s="17">
+        <v>2</v>
+      </c>
+      <c r="J65" s="17">
+        <v>2</v>
+      </c>
+      <c r="N65" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O65" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A66" s="2">
+        <v>65</v>
+      </c>
+      <c r="B66" s="18">
+        <v>9</v>
+      </c>
+      <c r="C66" s="18">
+        <v>0</v>
+      </c>
+      <c r="D66" s="18">
+        <v>0</v>
+      </c>
+      <c r="E66" s="18">
+        <v>1</v>
+      </c>
+      <c r="F66" s="18">
+        <v>10</v>
+      </c>
+      <c r="G66" s="18">
+        <v>3</v>
+      </c>
+      <c r="H66" s="18">
+        <v>3</v>
+      </c>
+      <c r="I66" s="18">
+        <v>2</v>
+      </c>
+      <c r="J66" s="18">
+        <v>3</v>
+      </c>
+      <c r="N66" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O66" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A67" s="2">
+        <v>66</v>
+      </c>
+      <c r="B67" s="18">
+        <v>1</v>
+      </c>
+      <c r="C67" s="18">
+        <v>0</v>
+      </c>
+      <c r="D67" s="18">
+        <v>2</v>
+      </c>
+      <c r="E67" s="18">
+        <v>1</v>
+      </c>
+      <c r="F67" s="18">
+        <v>2</v>
+      </c>
+      <c r="G67" s="18">
+        <v>3</v>
+      </c>
+      <c r="H67" s="18">
+        <v>3</v>
+      </c>
+      <c r="I67" s="18">
+        <v>3</v>
+      </c>
+      <c r="J67" s="18">
+        <v>3</v>
+      </c>
+      <c r="N67" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O67" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A68" s="2">
+        <v>67</v>
+      </c>
+      <c r="B68" s="20">
+        <v>98</v>
+      </c>
+      <c r="C68" s="19">
+        <v>3</v>
+      </c>
+      <c r="D68" s="19">
+        <v>4</v>
+      </c>
+      <c r="E68" s="20"/>
+      <c r="F68" s="20">
+        <v>2</v>
+      </c>
+      <c r="G68" s="20">
+        <v>1</v>
+      </c>
+      <c r="H68" s="20">
+        <v>2</v>
+      </c>
+      <c r="I68" s="20">
+        <v>2</v>
+      </c>
+      <c r="J68" s="20">
+        <v>3</v>
+      </c>
+      <c r="N68" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O68" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A69" s="2">
+        <v>68</v>
+      </c>
+      <c r="B69" s="19">
+        <v>33</v>
+      </c>
+      <c r="C69" s="19">
+        <v>4</v>
+      </c>
+      <c r="D69" s="19">
+        <v>3</v>
+      </c>
+      <c r="E69" s="19">
+        <v>0</v>
+      </c>
+      <c r="F69" s="19">
+        <v>0</v>
+      </c>
+      <c r="G69" s="19">
+        <v>2</v>
+      </c>
+      <c r="H69" s="19">
+        <v>2</v>
+      </c>
+      <c r="I69" s="19">
+        <v>1</v>
+      </c>
+      <c r="J69" s="19">
+        <v>3</v>
+      </c>
+      <c r="N69" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O69" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A70" s="2">
+        <v>69</v>
+      </c>
+      <c r="B70" s="21">
+        <v>84</v>
+      </c>
+      <c r="C70" s="21">
+        <v>4</v>
+      </c>
+      <c r="D70" s="21">
+        <v>1</v>
+      </c>
+      <c r="E70" s="21">
+        <v>0</v>
+      </c>
+      <c r="F70" s="21">
+        <v>4</v>
+      </c>
+      <c r="G70" s="21">
+        <v>1</v>
+      </c>
+      <c r="H70" s="21">
+        <v>2</v>
+      </c>
+      <c r="I70" s="21">
+        <v>3</v>
+      </c>
+      <c r="J70" s="21">
+        <v>2</v>
+      </c>
+      <c r="N70" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O70" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A71" s="2">
+        <v>70</v>
+      </c>
+      <c r="B71" s="23">
+        <v>18</v>
+      </c>
+      <c r="C71" s="22">
+        <v>0</v>
+      </c>
+      <c r="D71" s="22">
+        <v>5</v>
+      </c>
+      <c r="E71" s="23">
+        <v>2</v>
+      </c>
+      <c r="F71" s="23">
+        <v>5</v>
+      </c>
+      <c r="G71" s="23">
+        <v>3</v>
+      </c>
+      <c r="H71" s="23">
+        <v>3</v>
+      </c>
+      <c r="I71" s="23">
+        <v>2</v>
+      </c>
+      <c r="J71" s="23">
+        <v>3</v>
+      </c>
+      <c r="K71" s="22">
+        <v>3</v>
+      </c>
+      <c r="N71" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O71" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A72" s="2">
+        <v>71</v>
+      </c>
+      <c r="B72" s="22">
+        <v>34</v>
+      </c>
+      <c r="C72" s="22">
+        <v>0</v>
+      </c>
+      <c r="D72" s="22">
+        <v>1</v>
+      </c>
+      <c r="E72" s="22">
+        <v>0</v>
+      </c>
+      <c r="F72" s="22">
+        <v>7</v>
+      </c>
+      <c r="G72" s="22">
+        <v>3</v>
+      </c>
+      <c r="H72" s="22">
+        <v>3</v>
+      </c>
+      <c r="I72" s="22">
+        <v>3</v>
+      </c>
+      <c r="J72" s="22">
+        <v>3</v>
+      </c>
+      <c r="K72" s="22">
+        <v>1</v>
+      </c>
+      <c r="N72" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O72" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A73" s="2">
+        <v>72</v>
+      </c>
+      <c r="B73" s="22">
+        <v>325</v>
+      </c>
+      <c r="C73" s="22">
+        <v>5</v>
+      </c>
+      <c r="D73" s="22">
+        <v>11</v>
+      </c>
+      <c r="E73" s="22">
+        <v>1</v>
+      </c>
+      <c r="F73" s="22">
+        <v>10</v>
+      </c>
+      <c r="G73" s="22">
+        <v>1</v>
+      </c>
+      <c r="H73" s="22">
+        <v>3</v>
+      </c>
+      <c r="I73" s="22">
+        <v>1</v>
+      </c>
+      <c r="J73" s="22">
+        <v>1</v>
+      </c>
+      <c r="K73" s="22">
+        <v>1</v>
+      </c>
+      <c r="N73" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O73" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A74" s="2">
+        <v>73</v>
+      </c>
+      <c r="B74" s="22">
+        <v>27</v>
+      </c>
+      <c r="C74" s="22">
+        <v>0</v>
+      </c>
+      <c r="D74" s="22">
+        <v>2</v>
+      </c>
+      <c r="E74" s="22">
+        <v>0</v>
+      </c>
+      <c r="F74" s="22">
+        <v>3</v>
+      </c>
+      <c r="G74" s="22">
+        <v>3</v>
+      </c>
+      <c r="H74" s="22">
+        <v>3</v>
+      </c>
+      <c r="I74" s="22">
+        <v>3</v>
+      </c>
+      <c r="J74" s="22">
+        <v>3</v>
+      </c>
+      <c r="K74" s="22">
+        <v>3</v>
+      </c>
+      <c r="N74" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O74" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A75" s="2">
+        <v>74</v>
+      </c>
+      <c r="B75" s="24">
+        <v>11</v>
+      </c>
+      <c r="C75" s="24">
+        <v>0</v>
+      </c>
+      <c r="D75" s="24">
+        <v>0</v>
+      </c>
+      <c r="E75" s="24">
+        <v>2</v>
+      </c>
+      <c r="F75" s="24">
+        <v>6</v>
+      </c>
+      <c r="G75" s="24">
+        <v>3</v>
+      </c>
+      <c r="H75" s="24">
+        <v>3</v>
+      </c>
+      <c r="I75" s="24">
+        <v>3</v>
+      </c>
+      <c r="J75" s="24">
+        <v>3</v>
+      </c>
+      <c r="K75" s="25">
+        <v>3</v>
+      </c>
+      <c r="N75" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O75" s="5" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>